<commit_message>
Criação do Manual do Usuário
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/HD - Checklist Verificacao de Projeto - Interno.xlsx
+++ b/Gerenciamento de Projeto/HD - Checklist Verificacao de Projeto - Interno.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22443F63-5289-4813-B11F-195336AF4AF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B47EA2-4B4F-4764-9586-86EAC68ECA86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -620,7 +620,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="136">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1560,7 +1560,7 @@
                   <c:v>0.80645161290322576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.80645161290322576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2076,9 +2076,9 @@
       <c r="A6" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="21" t="e">
+      <c r="B6" s="21">
         <f>'Ver-Transição1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.80645161290322576</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3503,7 +3503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -4228,17 +4228,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D49" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -4254,8 +4254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4288,9 +4288,9 @@
         <v>46</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="22" t="e">
+      <c r="F2" s="22">
         <f>COUNTIF(D5:D50,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.80645161290322576</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
@@ -4345,7 +4345,9 @@
       <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
@@ -4367,7 +4369,9 @@
       <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
@@ -4389,7 +4393,9 @@
       <c r="C10" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
@@ -4401,7 +4407,9 @@
       <c r="C11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -4413,7 +4421,9 @@
       <c r="C12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -4435,7 +4445,9 @@
       <c r="C14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
@@ -4457,7 +4469,9 @@
       <c r="C16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
@@ -4481,7 +4495,9 @@
       <c r="C18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
@@ -4505,7 +4521,9 @@
       <c r="C20" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -4517,7 +4535,9 @@
       <c r="C21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -4529,7 +4549,9 @@
       <c r="C22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
@@ -4541,7 +4563,9 @@
       <c r="C23" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
@@ -4553,7 +4577,9 @@
       <c r="C24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -4577,7 +4603,9 @@
       <c r="C26" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -4589,7 +4617,9 @@
       <c r="C27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -4601,7 +4631,9 @@
       <c r="C28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
@@ -4625,7 +4657,9 @@
       <c r="C30" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
@@ -4637,7 +4671,9 @@
       <c r="C31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -4659,7 +4695,9 @@
       <c r="C33" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -4671,7 +4709,9 @@
       <c r="C34" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -4695,7 +4735,9 @@
       <c r="C36" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
@@ -4707,7 +4749,9 @@
       <c r="C37" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -4719,7 +4763,9 @@
       <c r="C38" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -4731,7 +4777,9 @@
       <c r="C39" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -4743,7 +4791,9 @@
       <c r="C40" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
@@ -4755,7 +4805,9 @@
       <c r="C41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -4767,7 +4819,9 @@
       <c r="C42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
@@ -4791,7 +4845,9 @@
       <c r="C44" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
@@ -4803,7 +4859,9 @@
       <c r="C45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
@@ -4815,7 +4873,9 @@
       <c r="C46" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
@@ -4837,7 +4897,9 @@
       <c r="C48" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
@@ -4849,7 +4911,9 @@
       <c r="C49" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
@@ -4861,7 +4925,9 @@
       <c r="C50" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
@@ -4895,6 +4961,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -4902,11 +4973,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D48" xr:uid="{00000000-0002-0000-0400-000000000000}">

</xml_diff>